<commit_message>
votes per party per state
</commit_message>
<xml_diff>
--- a/flutter_application_1/assets/elecciones1994.xlsx
+++ b/flutter_application_1/assets/elecciones1994.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hansv\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABB9A02C-D1F1-4B23-99A0-7E7DFC08D92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5671979-E688-4A9E-A86E-F7B76656EA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54D397F3-039C-406B-BCC6-F1B78B6A6B55}"/>
   </bookViews>
@@ -1669,7 +1669,7 @@
   <dimension ref="A1:T301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>